<commit_message>
refactor: lat, long and time adjusted to DF logic
</commit_message>
<xml_diff>
--- a/data/GRARED_P_exemplo.xlsx
+++ b/data/GRARED_P_exemplo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\metpot04\Desktop\GIT\GRAREDv2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1DF258B-53B8-4673-A76D-0C1C7E3EA936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB8D9F7-80E8-4AE6-A558-2AC72016FE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GRARED_P_exemplo" sheetId="1" r:id="rId1"/>
@@ -43,32 +43,32 @@
     <t>h_instrumento</t>
   </si>
   <si>
-    <t>Lat_gra</t>
+    <t>alt_m</t>
   </si>
   <si>
-    <t>Lat_min</t>
+    <t>lat_gra</t>
   </si>
   <si>
-    <t>Lat_seg</t>
+    <t>lat_min</t>
   </si>
   <si>
-    <t>Lon_gra</t>
+    <t>lat_seg</t>
   </si>
   <si>
-    <t>Lon_min</t>
+    <t>lon_gra</t>
   </si>
   <si>
-    <t>Lon_seg</t>
+    <t>lon_min</t>
   </si>
   <si>
-    <t>alt_m</t>
+    <t>lon_seg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +199,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -545,8 +553,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -901,14 +910,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,28 +942,28 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -996,7 +1007,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1040,7 +1051,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1084,7 +1095,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1128,7 +1139,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1172,7 +1183,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1216,7 +1227,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1260,7 +1271,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1304,7 +1315,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1347,8 +1358,12 @@
       <c r="N10">
         <v>25</v>
       </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>